<commit_message>
Subiendo cambios del sistema de registro de arrestados
</commit_message>
<xml_diff>
--- a/data/registros.xlsx
+++ b/data/registros.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O10"/>
+  <dimension ref="A1:O15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,90 +436,88 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
+          <t>Nombre del Arrestado</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>CI</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Edad</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Ocupación</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Fecha y Hora de Ingreso</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
           <t>Motivo de la Detención</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Nombre del Arrestado</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Edad</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Ocupación</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>CI</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Estado Físico del Arrestado</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>Nombre del Funcionario Policial</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>Unidad</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>Estado Físico del Arrestado</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>Descripción de Objetos del Arrestado</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>Lugar donde fue Arrestado</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>Nombre del Denunciante</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
-        <is>
-          <t>Fecha y Hora de Ingreso</t>
-        </is>
-      </c>
       <c r="M1" s="1" t="inlineStr">
         <is>
+          <t>Fecha y Hora de Salida</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>Imagen</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
           <t>ID</t>
-        </is>
-      </c>
-      <c r="N1" s="1" t="inlineStr">
-        <is>
-          <t>Imagen</t>
-        </is>
-      </c>
-      <c r="O1" s="1" t="inlineStr">
-        <is>
-          <t>Fecha y Hora de Salida</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>robo</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
           <t>juan gallardo</t>
         </is>
+      </c>
+      <c r="B2" t="n">
+        <v>66666666</v>
       </c>
       <c r="C2" t="n">
         <v>27</v>
@@ -529,47 +527,49 @@
           <t>chofer</t>
         </is>
       </c>
-      <c r="E2" t="n">
-        <v>66666666</v>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>2025-04-25 11:24:41</t>
+        </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
+          <t>robo</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>normal</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
           <t>Sgto. vila</t>
         </is>
       </c>
-      <c r="G2" t="inlineStr">
+      <c r="I2" t="inlineStr">
         <is>
           <t>Conciliacion Ciudadana</t>
         </is>
       </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>normal</t>
-        </is>
-      </c>
-      <c r="I2" t="inlineStr">
+      <c r="J2" t="inlineStr">
         <is>
           <t>billetra, celular</t>
         </is>
       </c>
-      <c r="J2" t="inlineStr">
+      <c r="K2" t="inlineStr">
         <is>
           <t>cementerio general</t>
         </is>
       </c>
-      <c r="K2" t="inlineStr">
+      <c r="L2" t="inlineStr">
         <is>
           <t>vecinos</t>
         </is>
       </c>
-      <c r="L2" t="inlineStr">
-        <is>
-          <t>2025-04-25 11:24:41</t>
-        </is>
-      </c>
       <c r="M2" t="inlineStr">
         <is>
-          <t>33ef8def</t>
+          <t>2025-04-26 11:00:00</t>
         </is>
       </c>
       <c r="N2" t="inlineStr">
@@ -582,13 +582,11 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>robo</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
           <t>juan gallardo</t>
         </is>
+      </c>
+      <c r="B3" t="n">
+        <v>66666666</v>
       </c>
       <c r="C3" t="n">
         <v>27</v>
@@ -598,47 +596,49 @@
           <t>chofer</t>
         </is>
       </c>
-      <c r="E3" t="n">
-        <v>66666666</v>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>2025-04-25 11:24:49</t>
+        </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
+          <t>robo</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>normal</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
           <t>Sgto. vila</t>
         </is>
       </c>
-      <c r="G3" t="inlineStr">
+      <c r="I3" t="inlineStr">
         <is>
           <t>Conciliacion Ciudadana</t>
         </is>
       </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>normal</t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr">
+      <c r="J3" t="inlineStr">
         <is>
           <t>billetra, celular</t>
         </is>
       </c>
-      <c r="J3" t="inlineStr">
+      <c r="K3" t="inlineStr">
         <is>
           <t>cementerio general</t>
         </is>
       </c>
-      <c r="K3" t="inlineStr">
+      <c r="L3" t="inlineStr">
         <is>
           <t>vecinos</t>
         </is>
       </c>
-      <c r="L3" t="inlineStr">
-        <is>
-          <t>2025-04-25 11:24:49</t>
-        </is>
-      </c>
       <c r="M3" t="inlineStr">
         <is>
-          <t>121ecb93</t>
+          <t>2025-05-10 12:22:00</t>
         </is>
       </c>
       <c r="N3" t="inlineStr">
@@ -651,13 +651,11 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>pelea</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
           <t>ramiro gonzales</t>
         </is>
+      </c>
+      <c r="B4" t="n">
+        <v>66683373782</v>
       </c>
       <c r="C4" t="n">
         <v>55</v>
@@ -667,62 +665,66 @@
           <t>obrero</t>
         </is>
       </c>
-      <c r="E4" t="n">
-        <v>66683373782</v>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>2025-04-25 11:40:51</t>
+        </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
+          <t>peleas callejeras</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>golpeado</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
           <t>sgto. ala</t>
         </is>
       </c>
-      <c r="G4" t="inlineStr">
+      <c r="I4" t="inlineStr">
         <is>
           <t>Dpto. "II" Inteligencia</t>
         </is>
       </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>golpeado</t>
-        </is>
-      </c>
-      <c r="I4" t="inlineStr">
+      <c r="J4" t="inlineStr">
         <is>
           <t>celular</t>
         </is>
       </c>
-      <c r="J4" t="inlineStr">
+      <c r="K4" t="inlineStr">
         <is>
           <t>calle chayanta</t>
         </is>
       </c>
-      <c r="K4" t="inlineStr">
+      <c r="L4" t="inlineStr">
         <is>
           <t>anonimo</t>
         </is>
       </c>
-      <c r="L4" t="inlineStr">
-        <is>
-          <t>2025-04-25 11:40:51</t>
-        </is>
-      </c>
       <c r="M4" t="inlineStr">
         <is>
-          <t>8d72eeb5</t>
-        </is>
-      </c>
-      <c r="N4" t="inlineStr"/>
+          <t>2025-04-27 11:40:21</t>
+        </is>
+      </c>
+      <c r="N4" t="inlineStr">
+        <is>
+          <t>C:/Users/Adm/Pictures/hacker.jpg</t>
+        </is>
+      </c>
       <c r="O4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>peleas callejeras</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
           <t>pablo lozada</t>
         </is>
+      </c>
+      <c r="B5" t="n">
+        <v>999990000</v>
       </c>
       <c r="C5" t="n">
         <v>39</v>
@@ -732,47 +734,49 @@
           <t>obrero</t>
         </is>
       </c>
-      <c r="E5" t="n">
-        <v>999990000</v>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>2025-04-28 11:51:34</t>
+        </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
+          <t>peleas callejeras</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>en buen estado fisico</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
           <t>sgto. mendoza</t>
         </is>
       </c>
-      <c r="G5" t="inlineStr">
+      <c r="I5" t="inlineStr">
         <is>
           <t>Dir. Dptal. F.E.L.C-C</t>
         </is>
       </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>en buen estado fisico</t>
-        </is>
-      </c>
-      <c r="I5" t="inlineStr">
+      <c r="J5" t="inlineStr">
         <is>
           <t>billetera, celular</t>
         </is>
       </c>
-      <c r="J5" t="inlineStr">
+      <c r="K5" t="inlineStr">
         <is>
           <t>bustillos</t>
         </is>
       </c>
-      <c r="K5" t="inlineStr">
+      <c r="L5" t="inlineStr">
         <is>
           <t>anonimo</t>
         </is>
       </c>
-      <c r="L5" t="inlineStr">
-        <is>
-          <t>2025-04-28 11:51:34</t>
-        </is>
-      </c>
       <c r="M5" t="inlineStr">
         <is>
-          <t>e4cb769d</t>
+          <t>9/6/25</t>
         </is>
       </c>
       <c r="N5" t="inlineStr">
@@ -785,13 +789,11 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>pelea callejera</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
           <t>Jose David</t>
         </is>
+      </c>
+      <c r="B6" t="n">
+        <v>555555555</v>
       </c>
       <c r="C6" t="n">
         <v>26</v>
@@ -801,49 +803,47 @@
           <t>estudiante</t>
         </is>
       </c>
-      <c r="E6" t="n">
-        <v>555555555</v>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>2025-04-29 16:03:11</t>
+        </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
+          <t>peleas callejeras</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>en estado  normal</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
           <t>Sgto. Ramirez</t>
         </is>
       </c>
-      <c r="G6" t="inlineStr">
+      <c r="I6" t="inlineStr">
         <is>
           <t>Tribunal Disciplinario Dptal.</t>
         </is>
       </c>
-      <c r="H6" t="inlineStr">
-        <is>
-          <t>en estado  normal</t>
-        </is>
-      </c>
-      <c r="I6" t="inlineStr">
+      <c r="J6" t="inlineStr">
         <is>
           <t>celular</t>
         </is>
       </c>
-      <c r="J6" t="inlineStr">
+      <c r="K6" t="inlineStr">
         <is>
           <t>av. los pinos</t>
         </is>
       </c>
-      <c r="K6" t="inlineStr">
+      <c r="L6" t="inlineStr">
         <is>
           <t>anonimo</t>
         </is>
       </c>
-      <c r="L6" t="inlineStr">
-        <is>
-          <t>2025-04-29 16:03:11</t>
-        </is>
-      </c>
-      <c r="M6" t="inlineStr">
-        <is>
-          <t>3d17c6be</t>
-        </is>
-      </c>
+      <c r="M6" t="inlineStr"/>
       <c r="N6" t="inlineStr">
         <is>
           <t>C:/Users/Adm/Pictures/hacker.jpg</t>
@@ -854,13 +854,11 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>robo</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
           <t>Cristian</t>
         </is>
+      </c>
+      <c r="B7" t="n">
+        <v>555443533</v>
       </c>
       <c r="C7" t="n">
         <v>35</v>
@@ -870,47 +868,49 @@
           <t>minero</t>
         </is>
       </c>
-      <c r="E7" t="n">
-        <v>555443533</v>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>2026-04-29 16:42:35</t>
+        </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
+          <t>robo</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>con golpes en la cabeza</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
           <t>Sgto quezada</t>
         </is>
       </c>
-      <c r="G7" t="inlineStr">
+      <c r="I7" t="inlineStr">
         <is>
           <t>Dir. Dptal. DIPROVE</t>
         </is>
       </c>
-      <c r="H7" t="inlineStr">
-        <is>
-          <t>con golpes en la cabeza</t>
-        </is>
-      </c>
-      <c r="I7" t="inlineStr">
+      <c r="J7" t="inlineStr">
         <is>
           <t>billetera y 2 celulares</t>
         </is>
       </c>
-      <c r="J7" t="inlineStr">
+      <c r="K7" t="inlineStr">
         <is>
           <t>calle tumusla</t>
         </is>
       </c>
-      <c r="K7" t="inlineStr">
+      <c r="L7" t="inlineStr">
         <is>
           <t>anonimo</t>
         </is>
       </c>
-      <c r="L7" t="inlineStr">
-        <is>
-          <t>2025-04-29 16:42:35</t>
-        </is>
-      </c>
       <c r="M7" t="inlineStr">
         <is>
-          <t>0b2852f1</t>
+          <t>10/6/25</t>
         </is>
       </c>
       <c r="N7" t="inlineStr">
@@ -923,63 +923,63 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>pelea calleejera entre grupo dev estudiantes universitarios</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>Jose David Mamani Huarachi</t>
-        </is>
+          <t>Royer tapia</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>82727777</v>
       </c>
       <c r="C8" t="n">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>estudiante de contabilidad de finanzas</t>
-        </is>
-      </c>
-      <c r="E8" t="n">
-        <v>7875795797</v>
+          <t>ing de sistemas</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>2025-04-30 10:36:49</t>
+        </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>Sgto Aguilar Erika</t>
+          <t>consumo de bebidas alcoholicas</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>Dir. Dptal. DIPROVE</t>
+          <t>en estado normal</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>ematomas en el pie derecho</t>
+          <t>sgto.ramirex raul</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>mochila con cuaderno, auriculares , botella de agua, celular y billetera</t>
+          <t>JEDECEV</t>
         </is>
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>Calle Sucre</t>
+          <t>mochila, celular galaxy a11 con pantallla trizada de color azul , billetras de cuero de color cafe y con lineas rojas con ci, licencia de conducir, billete de 200 bs  y unas monedas que en total seria 8 bs</t>
         </is>
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>los vecinos de la calle</t>
+          <t>en plaza  San Roque</t>
         </is>
       </c>
       <c r="L8" t="inlineStr">
         <is>
-          <t>2025-04-29 16:53:03</t>
+          <t>vecinos de la zona</t>
         </is>
       </c>
       <c r="M8" t="inlineStr">
         <is>
-          <t>1f08c444</t>
+          <t>8/6/25</t>
         </is>
       </c>
       <c r="N8" t="inlineStr">
@@ -992,63 +992,63 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>consumo de bebidas alcoholicas en via publica</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>Royer tapia</t>
-        </is>
+          <t>edwin menacho</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>63639629</v>
       </c>
       <c r="C9" t="n">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>ing de sistemas</t>
-        </is>
-      </c>
-      <c r="E9" t="n">
-        <v>82727777</v>
+          <t>estudiante</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>2025-05-07 10:05:15</t>
+        </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>sgto.ramirex raul</t>
+          <t>consumo de bebidas alcoholicas</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>JEDECEV</t>
+          <t>en estado de ebriedad</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>en estado normal</t>
+          <t>Sgto. Ernesto Yucra</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>mochila, celular galaxy a11 con pantallla trizada de color azul , billetras de cuero de color cafe y con lineas rojas con ci, licencia de conducir, billete de 200 bs  y unas monedas que en total seria 8 bs</t>
+          <t>IITCUP</t>
         </is>
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>en plaza  San Roque</t>
+          <t>celular y billetera</t>
         </is>
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>vecinos de la zona</t>
+          <t>av las banderas</t>
         </is>
       </c>
       <c r="L9" t="inlineStr">
         <is>
-          <t>2025-04-30 10:36:49</t>
+          <t>vecinos</t>
         </is>
       </c>
       <c r="M9" t="inlineStr">
         <is>
-          <t>9dc672a8</t>
+          <t>5/6/25</t>
         </is>
       </c>
       <c r="N9" t="inlineStr">
@@ -1061,71 +1061,392 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>consumo de bebidas alcoholicas</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>edwin menacho</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>24</t>
-        </is>
+          <t>Alvaro Torrez</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>3992999990</v>
+      </c>
+      <c r="C10" t="n">
+        <v>38</v>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>estudiante</t>
+          <t>chofer</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>63639629</t>
+          <t>2025-05-28 16:14:12</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>Sgto. Ernesto Yucra</t>
+          <t>consumo de bebidas</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>IITCUP</t>
+          <t>normal</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>en estado de ebriedad</t>
+          <t>Sgt. Ramirez</t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
         <is>
+          <t>Dir. Dptal Bomberos</t>
+        </is>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>celular, billetera</t>
+        </is>
+      </c>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>calle sucre</t>
+        </is>
+      </c>
+      <c r="L10" t="inlineStr">
+        <is>
+          <t>anonimo</t>
+        </is>
+      </c>
+      <c r="M10" t="inlineStr">
+        <is>
+          <t>6/6/25</t>
+        </is>
+      </c>
+      <c r="N10" t="inlineStr">
+        <is>
+          <t>C:/Users/Adm/Pictures/hacker.jpg</t>
+        </is>
+      </c>
+      <c r="O10" t="inlineStr"/>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>juan</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>7788669</v>
+      </c>
+      <c r="C11" t="n">
+        <v>25</v>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>minero</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>2025-06-04 16:52:58</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>peleas callejeras</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>golpeado</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>sgto. alvares</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>Dpto. "III" PP.OO</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>celular</t>
+        </is>
+      </c>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t>karachipampa</t>
+        </is>
+      </c>
+      <c r="L11" t="inlineStr">
+        <is>
+          <t>nose</t>
+        </is>
+      </c>
+      <c r="M11" t="inlineStr"/>
+      <c r="N11" t="inlineStr"/>
+      <c r="O11" t="inlineStr"/>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Sergio Chavarria</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>36737855</v>
+      </c>
+      <c r="C12" t="n">
+        <v>25</v>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>minero</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>2025-06-04 16:56:05</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>peleas callejeras</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>moreton en el ojo j</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>sgto. Chavarria</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>Sof. Plana Mayor</t>
+        </is>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>celular, billetera</t>
+        </is>
+      </c>
+      <c r="K12" t="inlineStr">
+        <is>
+          <t>nose</t>
+        </is>
+      </c>
+      <c r="L12" t="inlineStr">
+        <is>
+          <t>nose</t>
+        </is>
+      </c>
+      <c r="M12" t="inlineStr">
+        <is>
+          <t>6/6/25</t>
+        </is>
+      </c>
+      <c r="N12" t="inlineStr"/>
+      <c r="O12" t="inlineStr"/>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>jsiiais</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>857867844</v>
+      </c>
+      <c r="C13" t="n">
+        <v>66</v>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>hahavbhfhdsbj</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>2025-06-08 12:01:51</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>hola</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>jdjs</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>njjjdj</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>Otros</t>
+        </is>
+      </c>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>jsjkskska</t>
+        </is>
+      </c>
+      <c r="K13" t="inlineStr">
+        <is>
+          <t>jajajakakkaks</t>
+        </is>
+      </c>
+      <c r="L13" t="inlineStr">
+        <is>
+          <t>sjjsksjjsjsj</t>
+        </is>
+      </c>
+      <c r="M13" t="inlineStr"/>
+      <c r="N13" t="inlineStr"/>
+      <c r="O13" t="inlineStr"/>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Juan Ramirez</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>6625257</v>
+      </c>
+      <c r="C14" t="n">
+        <v>34</v>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>Obrero</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>2025-06-08 15:32:01</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>Pelea Callejera</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>normal</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>Sgto. Cruz</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>Otros</t>
+        </is>
+      </c>
+      <c r="J14" t="inlineStr">
+        <is>
           <t>celular y billetera</t>
         </is>
       </c>
-      <c r="J10" t="inlineStr">
-        <is>
-          <t>av las banderas</t>
-        </is>
-      </c>
-      <c r="K10" t="inlineStr">
-        <is>
-          <t>vecinos</t>
-        </is>
-      </c>
-      <c r="L10" t="inlineStr">
-        <is>
-          <t>2025-05-07 10:05:15</t>
-        </is>
-      </c>
-      <c r="M10" t="inlineStr">
-        <is>
-          <t>08c896df</t>
-        </is>
-      </c>
-      <c r="N10" t="inlineStr"/>
-      <c r="O10" t="inlineStr"/>
+      <c r="K14" t="inlineStr">
+        <is>
+          <t>Calle Tumusla</t>
+        </is>
+      </c>
+      <c r="L14" t="inlineStr">
+        <is>
+          <t>anonima</t>
+        </is>
+      </c>
+      <c r="M14" t="inlineStr"/>
+      <c r="N14" t="inlineStr">
+        <is>
+          <t>C:/Users/Adm/Pictures/hacker.jpg</t>
+        </is>
+      </c>
+      <c r="O14" t="inlineStr"/>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>nose</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>777879999</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>23</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>nose</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>2025-06-10 13:50:39</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>nose</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>nose</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>jjsnsjjjj</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>Sof. Plana Mayor</t>
+        </is>
+      </c>
+      <c r="J15" t="inlineStr">
+        <is>
+          <t>nose</t>
+        </is>
+      </c>
+      <c r="K15" t="inlineStr">
+        <is>
+          <t>nose</t>
+        </is>
+      </c>
+      <c r="L15" t="inlineStr">
+        <is>
+          <t>anonimo</t>
+        </is>
+      </c>
+      <c r="M15" t="inlineStr"/>
+      <c r="N15" t="inlineStr"/>
+      <c r="O15" t="inlineStr">
+        <is>
+          <t>f0d3a72f</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Ultimas modificaciones y ajustes que se hizo en el diseño del sistema
</commit_message>
<xml_diff>
--- a/data/registros.xlsx
+++ b/data/registros.xlsx
@@ -7,7 +7,8 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="2025" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O15"/>
+  <dimension ref="A1:O7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -513,14 +514,14 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>juan gallardo</t>
+          <t>Franz Catari Chavarria</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>66666666</v>
+        <v>66666677</v>
       </c>
       <c r="C2" t="n">
-        <v>27</v>
+        <v>56</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
@@ -529,37 +530,37 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>2025-04-25 11:24:41</t>
+          <t>2025-06-11 17:21:44</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>robo</t>
+          <t>pelea en via publica</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>normal</t>
+          <t>pequeñas lesiones en la cara</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>Sgto. vila</t>
+          <t>Sgto Soliz</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>Conciliacion Ciudadana</t>
+          <t>Dpto. "II" Inteligencia</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>billetra, celular</t>
+          <t>no tenia nada</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>cementerio general</t>
+          <t>carretera Sucre</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
@@ -569,7 +570,7 @@
       </c>
       <c r="M2" t="inlineStr">
         <is>
-          <t>2025-04-26 11:00:00</t>
+          <t>15/6/25</t>
         </is>
       </c>
       <c r="N2" t="inlineStr">
@@ -582,53 +583,53 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>juan gallardo</t>
+          <t>Sergio Chavarria Mayta</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>66666666</v>
+        <v>87479399</v>
       </c>
       <c r="C3" t="n">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>chofer</t>
+          <t>minero</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>2025-04-25 11:24:49</t>
+          <t>2025-06-12 18:27:59</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>robo</t>
+          <t>consumo de bebidas alcoholicas</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>normal</t>
+          <t>en estado de ebriedad</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>Sgto. vila</t>
+          <t>Sgto. Chavez</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>Conciliacion Ciudadana</t>
+          <t>Dir. Dptal. DIPROVE</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>billetra, celular</t>
+          <t>Celular, billetera</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>cementerio general</t>
+          <t>Av. Circunvalacion</t>
         </is>
       </c>
       <c r="L3" t="inlineStr">
@@ -638,7 +639,7 @@
       </c>
       <c r="M3" t="inlineStr">
         <is>
-          <t>2025-05-10 12:22:00</t>
+          <t>13/6/25</t>
         </is>
       </c>
       <c r="N3" t="inlineStr">
@@ -646,48 +647,52 @@
           <t>C:/Users/Adm/Pictures/hacker.jpg</t>
         </is>
       </c>
-      <c r="O3" t="inlineStr"/>
+      <c r="O3" t="inlineStr">
+        <is>
+          <t>112b817b</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>ramiro gonzales</t>
+          <t>Juan Valdez Mamani</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>66683373782</v>
+        <v>78980000</v>
       </c>
       <c r="C4" t="n">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>obrero</t>
+          <t>albañil</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>2025-04-25 11:40:51</t>
+          <t>2025-06-12 22:57:49</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>peleas callejeras</t>
+          <t>consumo de bebidas alcoholicas</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>golpeado</t>
+          <t>estado de ebriedad</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>sgto. ala</t>
+          <t>Sgto. Ramos</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>Dpto. "II" Inteligencia</t>
+          <t>DI.DI.PI</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
@@ -697,17 +702,17 @@
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>calle chayanta</t>
+          <t>calle Chayanta</t>
         </is>
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>anonimo</t>
+          <t>anonima</t>
         </is>
       </c>
       <c r="M4" t="inlineStr">
         <is>
-          <t>2025-04-27 11:40:21</t>
+          <t>15/6/25</t>
         </is>
       </c>
       <c r="N4" t="inlineStr">
@@ -715,68 +720,72 @@
           <t>C:/Users/Adm/Pictures/hacker.jpg</t>
         </is>
       </c>
-      <c r="O4" t="inlineStr"/>
+      <c r="O4" t="inlineStr">
+        <is>
+          <t>13f0ea8a</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>pablo lozada</t>
+          <t>Susana Muñoz Ramirez</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>999990000</v>
+        <v>9349993</v>
       </c>
       <c r="C5" t="n">
-        <v>39</v>
+        <v>23</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>obrero</t>
+          <t>estudiante</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>2025-04-28 11:51:34</t>
+          <t>2025-06-12 23:11:13</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>peleas callejeras</t>
+          <t>consumo de bebidas alcoholicas</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>en buen estado fisico</t>
+          <t>en estado de ebriedad</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>sgto. mendoza</t>
+          <t>Sgto. Villazon</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>Dir. Dptal. F.E.L.C-C</t>
+          <t>no se sabe</t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>billetera, celular</t>
+          <t>celular</t>
         </is>
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>bustillos</t>
+          <t>zona Villa Victoria</t>
         </is>
       </c>
       <c r="L5" t="inlineStr">
         <is>
-          <t>anonimo</t>
+          <t>anonima</t>
         </is>
       </c>
       <c r="M5" t="inlineStr">
         <is>
-          <t>9/6/25</t>
+          <t>15/6/25</t>
         </is>
       </c>
       <c r="N5" t="inlineStr">
@@ -784,19 +793,23 @@
           <t>C:/Users/Adm/Pictures/hacker.jpg</t>
         </is>
       </c>
-      <c r="O5" t="inlineStr"/>
+      <c r="O5" t="inlineStr">
+        <is>
+          <t>9c6814e8</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Jose David</t>
+          <t>Leonardo Manrique Cruz</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>555555555</v>
+        <v>6666665</v>
       </c>
       <c r="C6" t="n">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
@@ -805,22 +818,22 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>2025-04-29 16:03:11</t>
+          <t>2025-06-13 01:21:34</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>peleas callejeras</t>
+          <t>pelea en via publica</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>en estado  normal</t>
+          <t>normal</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>Sgto. Ramirez</t>
+          <t>Sgto. Torrez</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
@@ -830,12 +843,12 @@
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>celular</t>
+          <t>billetera, celular y mochila</t>
         </is>
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>av. los pinos</t>
+          <t>calle chayanta entre Boqueron</t>
         </is>
       </c>
       <c r="L6" t="inlineStr">
@@ -843,608 +856,307 @@
           <t>anonimo</t>
         </is>
       </c>
-      <c r="M6" t="inlineStr"/>
+      <c r="M6" t="inlineStr">
+        <is>
+          <t>15/6/25</t>
+        </is>
+      </c>
       <c r="N6" t="inlineStr">
         <is>
           <t>C:/Users/Adm/Pictures/hacker.jpg</t>
         </is>
       </c>
-      <c r="O6" t="inlineStr"/>
+      <c r="O6" t="inlineStr">
+        <is>
+          <t>1d145bc4</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Cristian</t>
+          <t>Luis Choque Mamani</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>555443533</v>
+        <v>7362882</v>
       </c>
       <c r="C7" t="n">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>minero</t>
+          <t>obrero</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>2026-04-29 16:42:35</t>
+          <t>2025-06-13 09:54:10</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>robo</t>
+          <t>pelea en via publica</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>con golpes en la cabeza</t>
+          <t>normal</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>Sgto quezada</t>
+          <t>Sgto. Perez</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>Dir. Dptal. DIPROVE</t>
+          <t>Dir. Dptal. F.E.L.C-C</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>billetera y 2 celulares</t>
+          <t>billetera</t>
         </is>
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>calle tumusla</t>
+          <t>calle bustillos</t>
         </is>
       </c>
       <c r="L7" t="inlineStr">
         <is>
+          <t>anonima</t>
+        </is>
+      </c>
+      <c r="M7" t="inlineStr">
+        <is>
+          <t>15/6/25</t>
+        </is>
+      </c>
+      <c r="N7" t="inlineStr"/>
+      <c r="O7" t="inlineStr">
+        <is>
+          <t>aea9b4e6</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:N3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Nombre del Arrestado</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>CI</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Edad</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Ocupación</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Fecha y Hora de Ingreso</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Motivo de la Detención</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Estado Físico del Arrestado</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Nombre del Funcionario Policial</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Unidad</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>Descripción de Objetos del Arrestado</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>Lugar donde fue Arrestado</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>Nombre del Denunciante</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>Fecha y Hora de Salida</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>Imagen</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Franz Catari</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>66666677</v>
+      </c>
+      <c r="C2" t="n">
+        <v>56</v>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>chofer</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>2025-06-11 17:21:44</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>pelea</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>pequeñas lesiones en la cara</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>Sgto Soliz</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>Dpto. "II" Inteligencia</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>no tenia nada</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>carretera de Karachipampa</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>vecinos</t>
+        </is>
+      </c>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>12/6/25</t>
+        </is>
+      </c>
+      <c r="N2" t="inlineStr"/>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Mauricio Muñoz</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>67288999</v>
+      </c>
+      <c r="C3" t="n">
+        <v>25</v>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>estudiante</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>2025-06-11 17:26:39</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>consumo de bebidas alcoholicas</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>en estado de ebriedad</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>Sgto. Aguilar</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>Conciliacion Ciudadana</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>celular y billetera</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>plaza central</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
           <t>anonimo</t>
         </is>
       </c>
-      <c r="M7" t="inlineStr">
-        <is>
-          <t>10/6/25</t>
-        </is>
-      </c>
-      <c r="N7" t="inlineStr">
+      <c r="M3" t="inlineStr"/>
+      <c r="N3" t="inlineStr">
         <is>
           <t>C:/Users/Adm/Pictures/hacker.jpg</t>
-        </is>
-      </c>
-      <c r="O7" t="inlineStr"/>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>Royer tapia</t>
-        </is>
-      </c>
-      <c r="B8" t="n">
-        <v>82727777</v>
-      </c>
-      <c r="C8" t="n">
-        <v>35</v>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>ing de sistemas</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>2025-04-30 10:36:49</t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>consumo de bebidas alcoholicas</t>
-        </is>
-      </c>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>en estado normal</t>
-        </is>
-      </c>
-      <c r="H8" t="inlineStr">
-        <is>
-          <t>sgto.ramirex raul</t>
-        </is>
-      </c>
-      <c r="I8" t="inlineStr">
-        <is>
-          <t>JEDECEV</t>
-        </is>
-      </c>
-      <c r="J8" t="inlineStr">
-        <is>
-          <t>mochila, celular galaxy a11 con pantallla trizada de color azul , billetras de cuero de color cafe y con lineas rojas con ci, licencia de conducir, billete de 200 bs  y unas monedas que en total seria 8 bs</t>
-        </is>
-      </c>
-      <c r="K8" t="inlineStr">
-        <is>
-          <t>en plaza  San Roque</t>
-        </is>
-      </c>
-      <c r="L8" t="inlineStr">
-        <is>
-          <t>vecinos de la zona</t>
-        </is>
-      </c>
-      <c r="M8" t="inlineStr">
-        <is>
-          <t>8/6/25</t>
-        </is>
-      </c>
-      <c r="N8" t="inlineStr">
-        <is>
-          <t>C:/Users/Adm/Pictures/hacker.jpg</t>
-        </is>
-      </c>
-      <c r="O8" t="inlineStr"/>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>edwin menacho</t>
-        </is>
-      </c>
-      <c r="B9" t="n">
-        <v>63639629</v>
-      </c>
-      <c r="C9" t="n">
-        <v>24</v>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>estudiante</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>2025-05-07 10:05:15</t>
-        </is>
-      </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>consumo de bebidas alcoholicas</t>
-        </is>
-      </c>
-      <c r="G9" t="inlineStr">
-        <is>
-          <t>en estado de ebriedad</t>
-        </is>
-      </c>
-      <c r="H9" t="inlineStr">
-        <is>
-          <t>Sgto. Ernesto Yucra</t>
-        </is>
-      </c>
-      <c r="I9" t="inlineStr">
-        <is>
-          <t>IITCUP</t>
-        </is>
-      </c>
-      <c r="J9" t="inlineStr">
-        <is>
-          <t>celular y billetera</t>
-        </is>
-      </c>
-      <c r="K9" t="inlineStr">
-        <is>
-          <t>av las banderas</t>
-        </is>
-      </c>
-      <c r="L9" t="inlineStr">
-        <is>
-          <t>vecinos</t>
-        </is>
-      </c>
-      <c r="M9" t="inlineStr">
-        <is>
-          <t>5/6/25</t>
-        </is>
-      </c>
-      <c r="N9" t="inlineStr">
-        <is>
-          <t>C:/Users/Adm/Pictures/hacker.jpg</t>
-        </is>
-      </c>
-      <c r="O9" t="inlineStr"/>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>Alvaro Torrez</t>
-        </is>
-      </c>
-      <c r="B10" t="n">
-        <v>3992999990</v>
-      </c>
-      <c r="C10" t="n">
-        <v>38</v>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>chofer</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>2025-05-28 16:14:12</t>
-        </is>
-      </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>consumo de bebidas</t>
-        </is>
-      </c>
-      <c r="G10" t="inlineStr">
-        <is>
-          <t>normal</t>
-        </is>
-      </c>
-      <c r="H10" t="inlineStr">
-        <is>
-          <t>Sgt. Ramirez</t>
-        </is>
-      </c>
-      <c r="I10" t="inlineStr">
-        <is>
-          <t>Dir. Dptal Bomberos</t>
-        </is>
-      </c>
-      <c r="J10" t="inlineStr">
-        <is>
-          <t>celular, billetera</t>
-        </is>
-      </c>
-      <c r="K10" t="inlineStr">
-        <is>
-          <t>calle sucre</t>
-        </is>
-      </c>
-      <c r="L10" t="inlineStr">
-        <is>
-          <t>anonimo</t>
-        </is>
-      </c>
-      <c r="M10" t="inlineStr">
-        <is>
-          <t>6/6/25</t>
-        </is>
-      </c>
-      <c r="N10" t="inlineStr">
-        <is>
-          <t>C:/Users/Adm/Pictures/hacker.jpg</t>
-        </is>
-      </c>
-      <c r="O10" t="inlineStr"/>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>juan</t>
-        </is>
-      </c>
-      <c r="B11" t="n">
-        <v>7788669</v>
-      </c>
-      <c r="C11" t="n">
-        <v>25</v>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>minero</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>2025-06-04 16:52:58</t>
-        </is>
-      </c>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>peleas callejeras</t>
-        </is>
-      </c>
-      <c r="G11" t="inlineStr">
-        <is>
-          <t>golpeado</t>
-        </is>
-      </c>
-      <c r="H11" t="inlineStr">
-        <is>
-          <t>sgto. alvares</t>
-        </is>
-      </c>
-      <c r="I11" t="inlineStr">
-        <is>
-          <t>Dpto. "III" PP.OO</t>
-        </is>
-      </c>
-      <c r="J11" t="inlineStr">
-        <is>
-          <t>celular</t>
-        </is>
-      </c>
-      <c r="K11" t="inlineStr">
-        <is>
-          <t>karachipampa</t>
-        </is>
-      </c>
-      <c r="L11" t="inlineStr">
-        <is>
-          <t>nose</t>
-        </is>
-      </c>
-      <c r="M11" t="inlineStr"/>
-      <c r="N11" t="inlineStr"/>
-      <c r="O11" t="inlineStr"/>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>Sergio Chavarria</t>
-        </is>
-      </c>
-      <c r="B12" t="n">
-        <v>36737855</v>
-      </c>
-      <c r="C12" t="n">
-        <v>25</v>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>minero</t>
-        </is>
-      </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>2025-06-04 16:56:05</t>
-        </is>
-      </c>
-      <c r="F12" t="inlineStr">
-        <is>
-          <t>peleas callejeras</t>
-        </is>
-      </c>
-      <c r="G12" t="inlineStr">
-        <is>
-          <t>moreton en el ojo j</t>
-        </is>
-      </c>
-      <c r="H12" t="inlineStr">
-        <is>
-          <t>sgto. Chavarria</t>
-        </is>
-      </c>
-      <c r="I12" t="inlineStr">
-        <is>
-          <t>Sof. Plana Mayor</t>
-        </is>
-      </c>
-      <c r="J12" t="inlineStr">
-        <is>
-          <t>celular, billetera</t>
-        </is>
-      </c>
-      <c r="K12" t="inlineStr">
-        <is>
-          <t>nose</t>
-        </is>
-      </c>
-      <c r="L12" t="inlineStr">
-        <is>
-          <t>nose</t>
-        </is>
-      </c>
-      <c r="M12" t="inlineStr">
-        <is>
-          <t>6/6/25</t>
-        </is>
-      </c>
-      <c r="N12" t="inlineStr"/>
-      <c r="O12" t="inlineStr"/>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>jsiiais</t>
-        </is>
-      </c>
-      <c r="B13" t="n">
-        <v>857867844</v>
-      </c>
-      <c r="C13" t="n">
-        <v>66</v>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>hahavbhfhdsbj</t>
-        </is>
-      </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>2025-06-08 12:01:51</t>
-        </is>
-      </c>
-      <c r="F13" t="inlineStr">
-        <is>
-          <t>hola</t>
-        </is>
-      </c>
-      <c r="G13" t="inlineStr">
-        <is>
-          <t>jdjs</t>
-        </is>
-      </c>
-      <c r="H13" t="inlineStr">
-        <is>
-          <t>njjjdj</t>
-        </is>
-      </c>
-      <c r="I13" t="inlineStr">
-        <is>
-          <t>Otros</t>
-        </is>
-      </c>
-      <c r="J13" t="inlineStr">
-        <is>
-          <t>jsjkskska</t>
-        </is>
-      </c>
-      <c r="K13" t="inlineStr">
-        <is>
-          <t>jajajakakkaks</t>
-        </is>
-      </c>
-      <c r="L13" t="inlineStr">
-        <is>
-          <t>sjjsksjjsjsj</t>
-        </is>
-      </c>
-      <c r="M13" t="inlineStr"/>
-      <c r="N13" t="inlineStr"/>
-      <c r="O13" t="inlineStr"/>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>Juan Ramirez</t>
-        </is>
-      </c>
-      <c r="B14" t="n">
-        <v>6625257</v>
-      </c>
-      <c r="C14" t="n">
-        <v>34</v>
-      </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>Obrero</t>
-        </is>
-      </c>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>2025-06-08 15:32:01</t>
-        </is>
-      </c>
-      <c r="F14" t="inlineStr">
-        <is>
-          <t>Pelea Callejera</t>
-        </is>
-      </c>
-      <c r="G14" t="inlineStr">
-        <is>
-          <t>normal</t>
-        </is>
-      </c>
-      <c r="H14" t="inlineStr">
-        <is>
-          <t>Sgto. Cruz</t>
-        </is>
-      </c>
-      <c r="I14" t="inlineStr">
-        <is>
-          <t>Otros</t>
-        </is>
-      </c>
-      <c r="J14" t="inlineStr">
-        <is>
-          <t>celular y billetera</t>
-        </is>
-      </c>
-      <c r="K14" t="inlineStr">
-        <is>
-          <t>Calle Tumusla</t>
-        </is>
-      </c>
-      <c r="L14" t="inlineStr">
-        <is>
-          <t>anonima</t>
-        </is>
-      </c>
-      <c r="M14" t="inlineStr"/>
-      <c r="N14" t="inlineStr">
-        <is>
-          <t>C:/Users/Adm/Pictures/hacker.jpg</t>
-        </is>
-      </c>
-      <c r="O14" t="inlineStr"/>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>nose</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>777879999</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>23</t>
-        </is>
-      </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>nose</t>
-        </is>
-      </c>
-      <c r="E15" t="inlineStr">
-        <is>
-          <t>2025-06-10 13:50:39</t>
-        </is>
-      </c>
-      <c r="F15" t="inlineStr">
-        <is>
-          <t>nose</t>
-        </is>
-      </c>
-      <c r="G15" t="inlineStr">
-        <is>
-          <t>nose</t>
-        </is>
-      </c>
-      <c r="H15" t="inlineStr">
-        <is>
-          <t>jjsnsjjjj</t>
-        </is>
-      </c>
-      <c r="I15" t="inlineStr">
-        <is>
-          <t>Sof. Plana Mayor</t>
-        </is>
-      </c>
-      <c r="J15" t="inlineStr">
-        <is>
-          <t>nose</t>
-        </is>
-      </c>
-      <c r="K15" t="inlineStr">
-        <is>
-          <t>nose</t>
-        </is>
-      </c>
-      <c r="L15" t="inlineStr">
-        <is>
-          <t>anonimo</t>
-        </is>
-      </c>
-      <c r="M15" t="inlineStr"/>
-      <c r="N15" t="inlineStr"/>
-      <c r="O15" t="inlineStr">
-        <is>
-          <t>f0d3a72f</t>
         </is>
       </c>
     </row>

</xml_diff>